<commit_message>
By Paul Leys, 2016-06-20.
   MD5: 83fe282521a21666e72d4bc77626dd96
 SHA-1: 2a51a9f386dfb4c630d6ed7069dd9a4c190d1397
</commit_message>
<xml_diff>
--- a/data_dictionary.xlsx
+++ b/data_dictionary.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16828"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="11400" windowHeight="4755" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="11400" windowHeight="4752" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="IIA" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Auteur</author>
   </authors>
   <commentList>
     <comment ref="A27" authorId="0" shapeId="0">
@@ -35,7 +35,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>Auteur:</t>
         </r>
         <r>
           <rPr>
@@ -59,7 +59,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>Auteur:</t>
         </r>
         <r>
           <rPr>
@@ -84,7 +84,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>Auteur:</t>
         </r>
         <r>
           <rPr>
@@ -108,7 +108,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>Auteur:</t>
         </r>
         <r>
           <rPr>
@@ -132,7 +132,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>Auteur:</t>
         </r>
         <r>
           <rPr>
@@ -145,6 +145,30 @@
 EUF-ASUS:
 the following data is required in the paper format for the signatures - these might be only partly relevant
 </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Auteur</author>
+  </authors>
+  <commentList>
+    <comment ref="A10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Paul Leys: should we, for the sake of consistency, use sending institution here (instead of home)?</t>
         </r>
       </text>
     </comment>
@@ -1114,8 +1138,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1208,6 +1232,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1298,8 +1329,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1315,9 +1346,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1355,7 +1386,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1390,23 +1421,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1442,26 +1456,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1637,21 +1634,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.5703125" customWidth="1"/>
-    <col min="6" max="6" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.5546875" customWidth="1"/>
+    <col min="6" max="6" width="39.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1668,7 +1665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>129</v>
       </c>
@@ -1681,7 +1678,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>168</v>
       </c>
@@ -1692,7 +1689,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>139</v>
       </c>
@@ -1705,7 +1702,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>130</v>
       </c>
@@ -1718,7 +1715,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>134</v>
       </c>
@@ -1729,7 +1726,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>169</v>
       </c>
@@ -1742,7 +1739,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>140</v>
       </c>
@@ -1755,7 +1752,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>135</v>
       </c>
@@ -1768,7 +1765,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>162</v>
       </c>
@@ -1785,7 +1782,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>141</v>
       </c>
@@ -1798,7 +1795,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>142</v>
       </c>
@@ -1811,7 +1808,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>143</v>
       </c>
@@ -1824,7 +1821,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>144</v>
       </c>
@@ -1837,7 +1834,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>147</v>
       </c>
@@ -1850,7 +1847,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>176</v>
       </c>
@@ -1861,7 +1858,7 @@
       </c>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>145</v>
       </c>
@@ -1872,7 +1869,7 @@
       </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>148</v>
       </c>
@@ -1883,7 +1880,7 @@
       </c>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>177</v>
       </c>
@@ -1894,7 +1891,7 @@
       </c>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>146</v>
       </c>
@@ -1905,7 +1902,7 @@
       </c>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>149</v>
       </c>
@@ -1916,7 +1913,7 @@
       </c>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>178</v>
       </c>
@@ -1927,7 +1924,7 @@
       </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>152</v>
       </c>
@@ -1938,7 +1935,7 @@
       </c>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>153</v>
       </c>
@@ -1949,7 +1946,7 @@
       </c>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>154</v>
       </c>
@@ -1960,7 +1957,7 @@
       </c>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>155</v>
       </c>
@@ -1971,7 +1968,7 @@
       </c>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>156</v>
       </c>
@@ -1982,7 +1979,7 @@
       </c>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>157</v>
       </c>
@@ -1993,7 +1990,7 @@
       </c>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>158</v>
       </c>
@@ -2004,7 +2001,7 @@
       </c>
       <c r="E29" s="8"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>159</v>
       </c>
@@ -2015,7 +2012,7 @@
       </c>
       <c r="E30" s="8"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>160</v>
       </c>
@@ -2026,7 +2023,7 @@
       </c>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>131</v>
       </c>
@@ -2035,7 +2032,7 @@
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>132</v>
       </c>
@@ -2044,7 +2041,7 @@
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>133</v>
       </c>
@@ -2053,7 +2050,7 @@
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>136</v>
       </c>
@@ -2062,7 +2059,7 @@
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>137</v>
       </c>
@@ -2071,7 +2068,7 @@
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>138</v>
       </c>
@@ -2080,7 +2077,7 @@
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
     </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>179</v>
       </c>
@@ -2093,7 +2090,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>181</v>
       </c>
@@ -2106,7 +2103,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>180</v>
       </c>
@@ -2119,7 +2116,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>182</v>
       </c>
@@ -2132,7 +2129,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
         <v>183</v>
       </c>
@@ -2145,7 +2142,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>184</v>
       </c>
@@ -2158,7 +2155,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
         <v>185</v>
       </c>
@@ -2171,7 +2168,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>186</v>
       </c>
@@ -2184,7 +2181,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
         <v>187</v>
       </c>
@@ -2197,7 +2194,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
         <v>188</v>
       </c>
@@ -2210,7 +2207,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
         <v>201</v>
       </c>
@@ -2219,7 +2216,7 @@
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
         <v>202</v>
       </c>
@@ -2230,7 +2227,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
         <v>203</v>
       </c>
@@ -2238,7 +2235,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
         <v>204</v>
       </c>
@@ -2246,7 +2243,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
         <v>205</v>
       </c>
@@ -2254,7 +2251,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
         <v>206</v>
       </c>
@@ -2262,62 +2259,62 @@
         <v>210</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="8" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
         <v>223</v>
       </c>
@@ -2336,7 +2333,7 @@
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2348,7 +2345,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2358,23 +2355,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="8" customWidth="1"/>
     <col min="3" max="3" width="14" style="8" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="72.140625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="44.28515625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="55.5703125" style="8" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="8"/>
+    <col min="4" max="4" width="15.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="72.109375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="44.33203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="55.5546875" style="8" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2395,7 +2392,7 @@
       </c>
       <c r="G1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>22</v>
       </c>
@@ -2406,7 +2403,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
@@ -2420,7 +2417,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>24</v>
       </c>
@@ -2434,7 +2431,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -2451,7 +2448,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
@@ -2465,7 +2462,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -2479,7 +2476,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
@@ -2490,7 +2487,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
@@ -2504,7 +2501,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
@@ -2518,7 +2515,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
@@ -2532,7 +2529,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
@@ -2546,7 +2543,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>11</v>
       </c>
@@ -2560,7 +2557,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
@@ -2574,7 +2571,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>25</v>
       </c>
@@ -2585,7 +2582,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
@@ -2596,7 +2593,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>14</v>
       </c>
@@ -2607,7 +2604,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
@@ -2621,7 +2618,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>16</v>
       </c>
@@ -2635,7 +2632,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>17</v>
       </c>
@@ -2649,7 +2646,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>18</v>
       </c>
@@ -2663,7 +2660,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>19</v>
       </c>
@@ -2677,7 +2674,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>63</v>
       </c>
@@ -2688,7 +2685,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>20</v>
       </c>
@@ -2699,7 +2696,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>21</v>
       </c>
@@ -2710,7 +2707,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>127</v>
       </c>
@@ -2718,7 +2715,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>121</v>
       </c>
@@ -2726,7 +2723,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>72</v>
       </c>
@@ -2740,7 +2737,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>73</v>
       </c>
@@ -2754,7 +2751,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>74</v>
       </c>
@@ -2768,7 +2765,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>75</v>
       </c>
@@ -2782,7 +2779,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>46</v>
       </c>
@@ -2790,7 +2787,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>43</v>
       </c>
@@ -2801,7 +2798,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>44</v>
       </c>
@@ -2815,7 +2812,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>45</v>
       </c>
@@ -2826,7 +2823,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>122</v>
       </c>
@@ -2834,7 +2831,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>77</v>
       </c>
@@ -2848,7 +2845,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>78</v>
       </c>
@@ -2862,7 +2859,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>79</v>
       </c>
@@ -2876,7 +2873,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>80</v>
       </c>
@@ -2890,7 +2887,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>47</v>
       </c>
@@ -2899,7 +2896,7 @@
       </c>
       <c r="E41" s="9"/>
     </row>
-    <row r="42" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
         <v>48</v>
       </c>
@@ -2910,13 +2907,13 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C43" s="8" t="s">
         <v>93</v>
       </c>
       <c r="E43" s="9"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
         <v>49</v>
       </c>
@@ -2927,7 +2924,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>50</v>
       </c>
@@ -2938,7 +2935,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
         <v>51</v>
       </c>
@@ -2949,7 +2946,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
         <v>52</v>
       </c>
@@ -2960,7 +2957,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
         <v>53</v>
       </c>
@@ -2971,7 +2968,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
         <v>54</v>
       </c>
@@ -2982,7 +2979,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
         <v>55</v>
       </c>
@@ -2993,7 +2990,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
         <v>56</v>
       </c>
@@ -3004,7 +3001,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
         <v>57</v>
       </c>
@@ -3015,7 +3012,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
         <v>118</v>
       </c>
@@ -3041,16 +3038,16 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3067,75 +3064,75 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>58</v>
       </c>
@@ -3146,24 +3143,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="61.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="3"/>
+    <col min="1" max="1" width="33.88671875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="61.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="3"/>
     <col min="5" max="5" width="46" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="3"/>
+    <col min="6" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3177,7 +3174,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>263</v>
       </c>
@@ -3188,7 +3185,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>264</v>
       </c>
@@ -3199,7 +3196,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>276</v>
       </c>
@@ -3207,7 +3204,7 @@
       <c r="D4"/>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>275</v>
       </c>
@@ -3215,7 +3212,7 @@
       <c r="D5"/>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>274</v>
       </c>
@@ -3225,7 +3222,7 @@
       <c r="D6"/>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>270</v>
       </c>
@@ -3235,7 +3232,7 @@
       <c r="D7"/>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>273</v>
       </c>
@@ -3245,7 +3242,7 @@
       <c r="D8"/>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>265</v>
       </c>
@@ -3253,7 +3250,7 @@
       <c r="D9"/>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>268</v>
       </c>
@@ -3261,37 +3258,37 @@
       <c r="D10"/>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>266</v>
       </c>
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>267</v>
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>272</v>
       </c>
       <c r="E13"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>271</v>
       </c>
       <c r="E14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>270</v>
       </c>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>269</v>
       </c>
@@ -3300,7 +3297,7 @@
       </c>
       <c r="E16"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>265</v>
       </c>
@@ -3308,11 +3305,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3324,17 +3322,17 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="107.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="107.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3352,7 +3350,7 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>224</v>
       </c>
@@ -3364,7 +3362,7 @@
       </c>
       <c r="F2" s="16"/>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>225</v>
       </c>
@@ -3376,7 +3374,7 @@
       </c>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>226</v>
       </c>
@@ -3388,7 +3386,7 @@
       </c>
       <c r="F4" s="16"/>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>231</v>
       </c>
@@ -3399,7 +3397,7 @@
       </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>232</v>
       </c>
@@ -3411,7 +3409,7 @@
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>233</v>
       </c>
@@ -3423,7 +3421,7 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>234</v>
       </c>
@@ -3435,7 +3433,7 @@
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>235</v>
       </c>
@@ -3447,7 +3445,7 @@
       </c>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>236</v>
       </c>
@@ -3459,7 +3457,7 @@
       </c>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>237</v>
       </c>
@@ -3471,7 +3469,7 @@
       </c>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>245</v>
       </c>
@@ -3483,7 +3481,7 @@
       </c>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>246</v>
       </c>
@@ -3495,7 +3493,7 @@
       </c>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>247</v>
       </c>
@@ -3507,7 +3505,7 @@
       </c>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>248</v>
       </c>
@@ -3519,7 +3517,7 @@
       </c>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>249</v>
       </c>
@@ -3531,7 +3529,7 @@
       </c>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>250</v>
       </c>
@@ -3543,7 +3541,7 @@
       </c>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>257</v>
       </c>
@@ -3555,7 +3553,7 @@
       </c>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -3563,7 +3561,7 @@
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -3571,7 +3569,7 @@
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -3579,7 +3577,7 @@
       <c r="E21" s="9"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -3587,7 +3585,7 @@
       <c r="E22" s="9"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -3595,7 +3593,7 @@
       <c r="E23" s="10"/>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -3603,7 +3601,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -3611,7 +3609,7 @@
       <c r="E25" s="9"/>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -3619,7 +3617,7 @@
       <c r="E26" s="9"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -3627,7 +3625,7 @@
       <c r="E27" s="9"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -3635,7 +3633,7 @@
       <c r="E28" s="9"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -3643,7 +3641,7 @@
       <c r="E29" s="9"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -3656,7 +3654,7 @@
       <c r="J30" s="14"/>
       <c r="K30" s="14"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -3669,7 +3667,7 @@
       <c r="J31" s="14"/>
       <c r="K31" s="14"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -3682,7 +3680,7 @@
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -3695,7 +3693,7 @@
       <c r="J33" s="14"/>
       <c r="K33" s="14"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -3708,7 +3706,7 @@
       <c r="J34" s="14"/>
       <c r="K34" s="14"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -3721,7 +3719,7 @@
       <c r="J35" s="14"/>
       <c r="K35" s="14"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -3734,7 +3732,7 @@
       <c r="J36" s="14"/>
       <c r="K36" s="14"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -3747,7 +3745,7 @@
       <c r="J37" s="14"/>
       <c r="K37" s="14"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -3760,7 +3758,7 @@
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -3773,7 +3771,7 @@
       <c r="J39" s="14"/>
       <c r="K39" s="14"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -3786,7 +3784,7 @@
       <c r="J40" s="14"/>
       <c r="K40" s="14"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -3799,7 +3797,7 @@
       <c r="J41" s="14"/>
       <c r="K41" s="14"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -3812,7 +3810,7 @@
       <c r="J42" s="14"/>
       <c r="K42" s="14"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -3825,7 +3823,7 @@
       <c r="J43" s="14"/>
       <c r="K43" s="14"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -3833,7 +3831,7 @@
       <c r="E44" s="9"/>
       <c r="F44" s="8"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -3841,7 +3839,7 @@
       <c r="E45" s="9"/>
       <c r="F45" s="8"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -3849,7 +3847,7 @@
       <c r="E46" s="9"/>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
@@ -3857,7 +3855,7 @@
       <c r="E47" s="9"/>
       <c r="F47" s="8"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -3865,7 +3863,7 @@
       <c r="E48" s="9"/>
       <c r="F48" s="8"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -3873,7 +3871,7 @@
       <c r="E49" s="9"/>
       <c r="F49" s="8"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
@@ -3881,7 +3879,7 @@
       <c r="E50" s="9"/>
       <c r="F50" s="8"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
@@ -3889,7 +3887,7 @@
       <c r="E51" s="9"/>
       <c r="F51" s="8"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
@@ -3897,7 +3895,7 @@
       <c r="E52" s="9"/>
       <c r="F52" s="8"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>

</xml_diff>

<commit_message>
Added color-coded WP3 columns (red = questions/potential problems, blue = tentative/naming difference)
</commit_message>
<xml_diff>
--- a/data_dictionary.xlsx
+++ b/data_dictionary.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="11400" windowHeight="4752" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="11400" windowHeight="4755" tabRatio="739"/>
   </bookViews>
   <sheets>
     <sheet name="IIA" sheetId="4" r:id="rId1"/>
@@ -15,17 +15,17 @@
     <sheet name="Transcript of Records" sheetId="2" r:id="rId6"/>
     <sheet name="Grade Conversion" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Auteur</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A27" authorId="0" shapeId="0">
+    <comment ref="A27" authorId="0">
       <text>
         <r>
           <rPr>
@@ -35,7 +35,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -49,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A32" authorId="0" shapeId="0">
+    <comment ref="A32" authorId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +59,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A41" authorId="0" shapeId="0">
+    <comment ref="A41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +84,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -98,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C42" authorId="0" shapeId="0">
+    <comment ref="E42" authorId="0">
       <text>
         <r>
           <rPr>
@@ -108,7 +108,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -122,7 +122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A44" authorId="0" shapeId="0">
+    <comment ref="A44" authorId="0">
       <text>
         <r>
           <rPr>
@@ -132,7 +132,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -155,10 +155,10 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Auteur</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A10" authorId="0" shapeId="0">
+    <comment ref="A10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -177,7 +177,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="362">
   <si>
     <t>Field Name</t>
   </si>
@@ -1134,12 +1134,234 @@
   <si>
     <t>[change_sending_added_component]</t>
   </si>
+  <si>
+    <t>Other Id (erasmus)</t>
+  </si>
+  <si>
+    <t>Start/End Date</t>
+  </si>
+  <si>
+    <t>ISCED Code</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>EQF Level</t>
+  </si>
+  <si>
+    <t>Mobility No (total)</t>
+  </si>
+  <si>
+    <t>Mobility No (average)</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Person ID</t>
+  </si>
+  <si>
+    <t>First Names</t>
+  </si>
+  <si>
+    <t>Birth Date</t>
+  </si>
+  <si>
+    <t>Citizenship</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>First/Last Name(s)</t>
+  </si>
+  <si>
+    <t>Not in model</t>
+  </si>
+  <si>
+    <t>LOS Code</t>
+  </si>
+  <si>
+    <t>Inst/Org Unit</t>
+  </si>
+  <si>
+    <t>IIA</t>
+  </si>
+  <si>
+    <t>Cooperation Condition</t>
+  </si>
+  <si>
+    <t>WP3 - Entity</t>
+  </si>
+  <si>
+    <t>WP3 - Attribute</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Mobility</t>
+  </si>
+  <si>
+    <t>Learning Opp Spec</t>
+  </si>
+  <si>
+    <t>Term Name</t>
+  </si>
+  <si>
+    <t>Learning Opp Inst</t>
+  </si>
+  <si>
+    <t>Credits (Scheme)</t>
+  </si>
+  <si>
+    <t>URL (Course Catalogue)</t>
+  </si>
+  <si>
+    <t>In Learning Agreement?</t>
+  </si>
+  <si>
+    <t>Not comp. list?</t>
+  </si>
+  <si>
+    <t>Not IIA?</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Arrival Date?</t>
+  </si>
+  <si>
+    <t>Departure Date?</t>
+  </si>
+  <si>
+    <t>Xxxx Component</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Credits</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Other Id (local)?</t>
+  </si>
+  <si>
+    <t>Contact Info</t>
+  </si>
+  <si>
+    <t>HEI Contact Info</t>
+  </si>
+  <si>
+    <t>Academic Year Name</t>
+  </si>
+  <si>
+    <t>Academic Term/Year</t>
+  </si>
+  <si>
+    <t>Academic Term</t>
+  </si>
+  <si>
+    <t>Result Distribution</t>
+  </si>
+  <si>
+    <t>1. Result Distribution      2. Learning Opp Spec</t>
+  </si>
+  <si>
+    <t>1. Label, (LOS Code)        2. Grading Scheme</t>
+  </si>
+  <si>
+    <t>Name (en)</t>
+  </si>
+  <si>
+    <t>Name (*)</t>
+  </si>
+  <si>
+    <t>Label, Count</t>
+  </si>
+  <si>
+    <t>Start/End Date?</t>
+  </si>
+  <si>
+    <t>Contact info (email)</t>
+  </si>
+  <si>
+    <t>Contact Info (phone)</t>
+  </si>
+  <si>
+    <t>Contact Info (url)</t>
+  </si>
+  <si>
+    <t>Contact Info (email)</t>
+  </si>
+  <si>
+    <t>to the</t>
+  </si>
+  <si>
+    <t>IIA level?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These are only </t>
+  </si>
+  <si>
+    <t>present on the</t>
+  </si>
+  <si>
+    <t>LOI level, but</t>
+  </si>
+  <si>
+    <t>can be aggregated</t>
+  </si>
+  <si>
+    <t>Academic Year Name, Start Date, End Date</t>
+  </si>
+  <si>
+    <t>Person Contact Info/Coordinator (role=visa)</t>
+  </si>
+  <si>
+    <t>HEI Contact Info (type=url, role=visa)</t>
+  </si>
+  <si>
+    <t>Person Contact Info/Coordinator (role=insurance)</t>
+  </si>
+  <si>
+    <t>HEI Contact Info (type=url, role=insurance)</t>
+  </si>
+  <si>
+    <t>Person Contact Info/Coordinator (role=housing)</t>
+  </si>
+  <si>
+    <t>HEI Contact Info (type=url, role=housing)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1239,6 +1461,27 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1277,7 +1520,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1326,14 +1569,42 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEB05A9"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1346,9 +1617,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1386,9 +1657,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1423,7 +1694,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1458,7 +1729,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1632,691 +1903,1056 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.5546875" customWidth="1"/>
-    <col min="6" max="6" width="39.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="24" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="73.5703125" customWidth="1"/>
+    <col min="8" max="8" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="22" t="s">
+        <v>314</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="23" t="s">
+        <v>291</v>
+      </c>
       <c r="C2" s="8" t="s">
-        <v>93</v>
+        <v>310</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
+      <c r="B3" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>310</v>
+      </c>
       <c r="D3" s="8"/>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="23" t="s">
+        <v>292</v>
+      </c>
       <c r="C4" s="8" t="s">
-        <v>93</v>
+        <v>310</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="21" t="s">
+        <v>288</v>
+      </c>
       <c r="C5" s="8" t="s">
-        <v>93</v>
+        <v>310</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
+      <c r="B6" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>310</v>
+      </c>
       <c r="D6" s="8"/>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="23" t="s">
+        <v>291</v>
+      </c>
       <c r="C7" s="8" t="s">
-        <v>93</v>
+        <v>310</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="23" t="s">
+        <v>292</v>
+      </c>
       <c r="C8" s="8" t="s">
-        <v>93</v>
+        <v>310</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8" t="s">
+      <c r="B9" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="G9" s="8" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="G10" s="8" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8" t="s">
+      <c r="B11" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="21" t="s">
+        <v>293</v>
+      </c>
       <c r="C12" s="8"/>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="G12" s="8" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8" t="s">
+      <c r="B13" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="20" t="s">
+        <v>297</v>
+      </c>
       <c r="C14" s="8"/>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="G14" s="8" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="11" t="s">
+      <c r="B15" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="G15" s="11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="11" t="s">
+      <c r="B16" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="B17" s="8"/>
+      <c r="B17" s="20" t="s">
+        <v>297</v>
+      </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="11" t="s">
+      <c r="B18" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="11" t="s">
+      <c r="B19" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B20" s="8"/>
+      <c r="B20" s="20" t="s">
+        <v>297</v>
+      </c>
       <c r="C20" s="8"/>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="11" t="s">
+      <c r="B21" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="11" t="s">
+      <c r="B22" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8" t="s">
+      <c r="B23" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="B24" s="8"/>
+      <c r="B24" s="21" t="s">
+        <v>293</v>
+      </c>
       <c r="C24" s="8"/>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8" t="s">
+      <c r="B25" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B26" s="8"/>
+      <c r="B26" s="20" t="s">
+        <v>297</v>
+      </c>
       <c r="C26" s="8"/>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8" t="s">
+      <c r="B27" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="B28" s="8"/>
+      <c r="B28" s="20" t="s">
+        <v>297</v>
+      </c>
       <c r="C28" s="8"/>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="E28" s="8"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8" t="s">
+      <c r="B29" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="B30" s="8"/>
+      <c r="B30" s="20" t="s">
+        <v>297</v>
+      </c>
       <c r="C30" s="8"/>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="E30" s="8"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8" t="s">
+      <c r="B31" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="E31" s="8"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G31" s="8"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
+      <c r="B32" s="23" t="s">
+        <v>345</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>334</v>
+      </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
+      <c r="B33" s="23" t="s">
+        <v>346</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>334</v>
+      </c>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
+      <c r="B34" s="21" t="s">
+        <v>347</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>334</v>
+      </c>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
+      <c r="B35" s="23" t="s">
+        <v>348</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>334</v>
+      </c>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
+      <c r="B36" s="23" t="s">
+        <v>346</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>334</v>
+      </c>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
+      <c r="B37" s="21" t="s">
+        <v>347</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>334</v>
+      </c>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+    </row>
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="B38" s="8"/>
+      <c r="B38" s="23" t="s">
+        <v>290</v>
+      </c>
       <c r="C38" s="8"/>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="G38" s="8" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8" t="s">
+      <c r="B39" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>352</v>
+      </c>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="G39" s="8" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8" t="s">
+      <c r="B40" s="30" t="s">
+        <v>353</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>354</v>
+      </c>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="G40" s="8" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8" t="s">
+      <c r="B41" s="30" t="s">
+        <v>349</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="G41" s="8" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="B42" s="8"/>
+      <c r="B42" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="C42" s="8"/>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="G42" s="8" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="B43" s="8"/>
+      <c r="B43" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="C43" s="8"/>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="G43" s="8" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="B44" s="8"/>
+      <c r="B44" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="C44" s="8"/>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="G44" s="8" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="B45" s="8"/>
+      <c r="B45" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="C45" s="8"/>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="G45" s="8" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="B46" s="8"/>
+      <c r="B46" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="C46" s="8"/>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="G46" s="8" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="B47" s="8"/>
+      <c r="B47" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="C47" s="8"/>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E47" s="8" t="s">
+      <c r="G47" s="8" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
+      <c r="B48" s="23" t="s">
+        <v>355</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>337</v>
+      </c>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+    </row>
+    <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="B49" s="23" t="s">
+        <v>355</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="G49" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="F49" t="s">
+      <c r="H49" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="B50" s="23" t="s">
+        <v>355</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="G50" s="8" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="B51" s="23" t="s">
+        <v>355</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="G51" s="8" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="B52" s="23" t="s">
+        <v>355</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="G52" s="8" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="B53" s="23" t="s">
+        <v>355</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="G53" s="8" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B54" s="23" t="s">
+        <v>333</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B55" s="23" t="s">
+        <v>333</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B56" s="23" t="s">
+        <v>333</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B57" s="23" t="s">
+        <v>333</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B58" s="23" t="s">
+        <v>333</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B59" s="23" t="s">
+        <v>333</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B60" s="23" t="s">
+        <v>333</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B61" s="23" t="s">
+        <v>333</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B62" s="23" t="s">
+        <v>333</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B63" s="23" t="s">
+        <v>333</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B64" s="23" t="s">
+        <v>333</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>223</v>
+      </c>
+      <c r="B65" s="23" t="s">
+        <v>333</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -2329,11 +2965,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2345,7 +2979,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2353,673 +2987,972 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="14" style="8" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="72.109375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="44.33203125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="55.5546875" style="8" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="8"/>
+    <col min="1" max="1" width="36.7109375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="23" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="23" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="14" style="8" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="72.140625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="44.28515625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="55.5703125" style="8" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="25" t="s">
+        <v>314</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="B2" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E3" s="9" t="s">
+      <c r="B3" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="B4" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="B6" s="21" t="s">
+        <v>305</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E7" s="9" t="s">
+      <c r="B7" s="23" t="s">
+        <v>300</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="H7" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="39" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E8" s="9" t="s">
+      <c r="B8" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>316</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E9" s="9" t="s">
+      <c r="B9" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>316</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="H9" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E10" s="9" t="s">
+      <c r="B10" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="H10" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E11" s="9" t="s">
+      <c r="B11" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="H11" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="39" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E12" s="9" t="s">
+      <c r="B12" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="H12" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E13" s="9" t="s">
+      <c r="B13" s="23" t="s">
+        <v>301</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="H13" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E14" s="9" t="s">
+      <c r="B14" s="23" t="s">
+        <v>292</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="H14" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E15" s="10" t="s">
+      <c r="B15" s="21" t="s">
+        <v>307</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E16" s="9" t="s">
+      <c r="B16" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E17" s="9" t="s">
+      <c r="B17" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E18" s="9" t="s">
+      <c r="B18" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="H18" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E19" s="9" t="s">
+      <c r="B19" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="H19" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="39" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E20" s="9" t="s">
+      <c r="B20" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="H20" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E21" s="9" t="s">
+      <c r="B21" s="23" t="s">
+        <v>301</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G21" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="H21" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E22" s="9" t="s">
+      <c r="B22" s="23" t="s">
+        <v>292</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G22" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="H22" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E23" s="10" t="s">
+      <c r="B23" s="21" t="s">
+        <v>307</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G23" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E24" s="9" t="s">
+      <c r="B24" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E25" s="9" t="s">
+      <c r="B25" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" s="9" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="B26" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>316</v>
+      </c>
+      <c r="G26" s="9" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="B27" s="20" t="s">
+        <v>308</v>
+      </c>
+      <c r="G27" s="9" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="8" t="s">
+      <c r="B28" s="21" t="s">
+        <v>309</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="G28" s="9" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D29" s="8" t="s">
+      <c r="B29" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="G29" s="9" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D30" s="8" t="s">
+      <c r="B30" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>319</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F30" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="G30" s="9" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" s="8" t="s">
+      <c r="B31" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>319</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="G31" s="9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="B32" s="23" t="s">
+        <v>293</v>
+      </c>
+      <c r="G32" s="9" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E33" s="9" t="s">
+      <c r="B33" s="21" t="s">
+        <v>321</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G33" s="9" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E34" s="9" t="s">
+      <c r="B34" s="20" t="s">
+        <v>322</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G34" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E35" s="9" t="s">
+      <c r="B35" s="20" t="s">
+        <v>322</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>324</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G35" s="9" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="B36" s="20" t="s">
+        <v>308</v>
+      </c>
+      <c r="G36" s="9" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D37" s="8" t="s">
+      <c r="B37" s="21" t="s">
+        <v>309</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F37" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="G37" s="9" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" s="8" t="s">
+      <c r="B38" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F38" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="G38" s="9" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D39" s="8" t="s">
+      <c r="B39" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>319</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F39" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="G39" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D40" s="8" t="s">
+      <c r="B40" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>319</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F40" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="G40" s="9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E41" s="9"/>
-    </row>
-    <row r="42" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B41" s="23" t="s">
+        <v>293</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G41" s="9"/>
+    </row>
+    <row r="42" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E42" s="9" t="s">
+      <c r="B42" s="20" t="s">
+        <v>308</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G42" s="9" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C43" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E43" s="9"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E43" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G43" s="9"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C44" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E44" s="9" t="s">
+      <c r="B44" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G44" s="9" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C45" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E45" s="9" t="s">
+      <c r="B45" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G45" s="9" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E46" s="9" t="s">
+      <c r="B46" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G46" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E47" s="9" t="s">
+      <c r="B47" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="C47" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G47" s="9" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C48" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E48" s="9" t="s">
+      <c r="B48" s="23" t="s">
+        <v>325</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G48" s="9" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E49" s="9" t="s">
+      <c r="B49" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="C49" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G49" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E50" s="9" t="s">
+      <c r="B50" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="C50" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G50" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C51" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E51" s="9" t="s">
+      <c r="B51" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="C51" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G51" s="9" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C52" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E52" s="9" t="s">
+      <c r="B52" s="23" t="s">
+        <v>325</v>
+      </c>
+      <c r="C52" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G52" s="9" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="C53" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E53" s="9" t="s">
+      <c r="B53" s="20" t="s">
+        <v>308</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G53" s="9" t="s">
         <v>119</v>
       </c>
     </row>
@@ -3038,16 +3971,16 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3064,75 +3997,75 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>58</v>
       </c>
@@ -3144,770 +4077,1047 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.88671875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="61.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="3"/>
-    <col min="5" max="5" width="46" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="3"/>
+    <col min="1" max="1" width="33.85546875" style="3" customWidth="1"/>
+    <col min="2" max="3" width="18.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="61.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="3"/>
+    <col min="7" max="7" width="46" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="25" t="s">
+        <v>314</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E2" t="s">
         <v>261</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E3" t="s">
         <v>262</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="C4"/>
-      <c r="D4"/>
+      <c r="B4" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>317</v>
+      </c>
       <c r="E4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4"/>
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="C5"/>
-      <c r="D5"/>
+      <c r="B5" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>317</v>
+      </c>
       <c r="E5"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5"/>
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="E6" t="s">
         <v>258</v>
       </c>
-      <c r="D6"/>
-      <c r="E6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6"/>
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="E7" t="s">
         <v>259</v>
       </c>
-      <c r="D7"/>
-      <c r="E7"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7"/>
+      <c r="G7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B8" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="E8" t="s">
         <v>260</v>
       </c>
-      <c r="D8"/>
-      <c r="E8"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8"/>
+      <c r="G8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="C9"/>
-      <c r="D9"/>
+      <c r="B9" s="27" t="s">
+        <v>293</v>
+      </c>
       <c r="E9"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9"/>
+      <c r="G9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="C10"/>
-      <c r="D10"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
       <c r="E10"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10"/>
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="E11"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="E12"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="E13"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="E14"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="E15"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="C16" t="s">
+      <c r="B16" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="E16" t="s">
         <v>277</v>
       </c>
-      <c r="E16"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="E17" t="s">
+      <c r="B17" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="G17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E18"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="107.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="107.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="25" t="s">
+        <v>314</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
+      <c r="B2" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>310</v>
+      </c>
       <c r="D2" s="16"/>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="F2" s="16"/>
-    </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
+      <c r="B3" s="29" t="s">
+        <v>332</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>310</v>
+      </c>
       <c r="D3" s="16"/>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="F3" s="16"/>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H3" s="16"/>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
+      <c r="B4" s="29" t="s">
+        <v>308</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>310</v>
+      </c>
       <c r="D4" s="16"/>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="F4" s="16"/>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="s">
+      <c r="B5" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
+      <c r="B6" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>310</v>
+      </c>
       <c r="D6" s="8"/>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+      <c r="B7" s="21" t="s">
+        <v>333</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>334</v>
+      </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="B8" s="21" t="s">
+        <v>333</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>334</v>
+      </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>336</v>
+      </c>
       <c r="D9" s="8"/>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="F9" s="8"/>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>337</v>
+      </c>
       <c r="D10" s="8"/>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="18" t="s">
         <v>242</v>
       </c>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>337</v>
+      </c>
       <c r="D11" s="8"/>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>339</v>
+      </c>
       <c r="D12" s="8"/>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+      <c r="B13" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>317</v>
+      </c>
       <c r="D13" s="8"/>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>317</v>
+      </c>
       <c r="D14" s="8"/>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
+      <c r="B15" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>317</v>
+      </c>
       <c r="D15" s="8"/>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
+      <c r="B16" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>317</v>
+      </c>
       <c r="D16" s="8"/>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+      <c r="B17" s="20" t="s">
+        <v>308</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>319</v>
+      </c>
       <c r="D17" s="8"/>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+      <c r="B18" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>338</v>
+      </c>
       <c r="D18" s="8"/>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H18" s="8"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="9"/>
+      <c r="E21" s="8"/>
       <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G21" s="9"/>
+      <c r="H21" s="8"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="9"/>
+      <c r="E22" s="8"/>
       <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G22" s="9"/>
+      <c r="H22" s="8"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="10"/>
+      <c r="E23" s="8"/>
       <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G23" s="10"/>
+      <c r="H23" s="8"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="9"/>
+      <c r="E24" s="8"/>
       <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G24" s="9"/>
+      <c r="H24" s="8"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="9"/>
+      <c r="E25" s="8"/>
       <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G25" s="9"/>
+      <c r="H25" s="8"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="9"/>
+      <c r="E26" s="8"/>
       <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G26" s="9"/>
+      <c r="H26" s="8"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="9"/>
+      <c r="E27" s="8"/>
       <c r="F27" s="8"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G27" s="9"/>
+      <c r="H27" s="8"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
-      <c r="E28" s="9"/>
+      <c r="E28" s="8"/>
       <c r="F28" s="8"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G28" s="9"/>
+      <c r="H28" s="8"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
-      <c r="E29" s="9"/>
+      <c r="E29" s="8"/>
       <c r="F29" s="8"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G29" s="9"/>
+      <c r="H29" s="8"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="13"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
       <c r="F30" s="12"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="12"/>
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
       <c r="K30" s="14"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="13"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
       <c r="F31" s="12"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="12"/>
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
       <c r="K31" s="14"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="13"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
       <c r="F32" s="12"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="12"/>
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="13"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
       <c r="F33" s="12"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="12"/>
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
       <c r="K33" s="14"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="15"/>
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
       <c r="K34" s="14"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="13"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
       <c r="F35" s="12"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="12"/>
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
       <c r="K35" s="14"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="13"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
       <c r="F36" s="12"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="12"/>
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
       <c r="K36" s="14"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="13"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
       <c r="F37" s="12"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="12"/>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
       <c r="K37" s="14"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="13"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
       <c r="F38" s="12"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="12"/>
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="13"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
       <c r="F39" s="12"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="12"/>
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
       <c r="K39" s="14"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="13"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
       <c r="F40" s="12"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="12"/>
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
       <c r="K40" s="14"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="13"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
       <c r="F41" s="12"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="12"/>
       <c r="I41" s="14"/>
       <c r="J41" s="14"/>
       <c r="K41" s="14"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="13"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
       <c r="F42" s="12"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="12"/>
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
       <c r="K42" s="14"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="13"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
       <c r="F43" s="12"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="12"/>
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
       <c r="K43" s="14"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
-      <c r="E44" s="9"/>
+      <c r="E44" s="8"/>
       <c r="F44" s="8"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G44" s="9"/>
+      <c r="H44" s="8"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
-      <c r="E45" s="9"/>
+      <c r="E45" s="8"/>
       <c r="F45" s="8"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G45" s="9"/>
+      <c r="H45" s="8"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
-      <c r="E46" s="9"/>
+      <c r="E46" s="8"/>
       <c r="F46" s="8"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G46" s="9"/>
+      <c r="H46" s="8"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
-      <c r="E47" s="9"/>
+      <c r="E47" s="8"/>
       <c r="F47" s="8"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G47" s="9"/>
+      <c r="H47" s="8"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
-      <c r="E48" s="9"/>
+      <c r="E48" s="8"/>
       <c r="F48" s="8"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G48" s="9"/>
+      <c r="H48" s="8"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
-      <c r="E49" s="9"/>
+      <c r="E49" s="8"/>
       <c r="F49" s="8"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49" s="9"/>
+      <c r="H49" s="8"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
-      <c r="E50" s="9"/>
+      <c r="E50" s="8"/>
       <c r="F50" s="8"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50" s="9"/>
+      <c r="H50" s="8"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
-      <c r="E51" s="9"/>
+      <c r="E51" s="8"/>
       <c r="F51" s="8"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51" s="9"/>
+      <c r="H51" s="8"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
-      <c r="E52" s="9"/>
+      <c r="E52" s="8"/>
       <c r="F52" s="8"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G52" s="9"/>
+      <c r="H52" s="8"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
-      <c r="E53" s="9"/>
+      <c r="E53" s="8"/>
       <c r="F53" s="8"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1" display="http://countrycode.org/"/>
-    <hyperlink ref="E12" r:id="rId2" display="http://egracons.eu/document/grading-table-instructions-and-template"/>
-    <hyperlink ref="E16" r:id="rId3" display="mailto:valere.meus@ugent.be?subject=Egracons%20project:%20more%20info%20needed"/>
+    <hyperlink ref="G6" r:id="rId1" display="http://countrycode.org/"/>
+    <hyperlink ref="G12" r:id="rId2" display="http://egracons.eu/document/grading-table-instructions-and-template"/>
+    <hyperlink ref="G16" r:id="rId3" display="mailto:valere.meus@ugent.be?subject=Egracons%20project:%20more%20info%20needed"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>